<commit_message>
versao com testes corrigidos
</commit_message>
<xml_diff>
--- a/code_smell_detection/Code_Smells_Testes.xlsx
+++ b/code_smell_detection/Code_Smells_Testes.xlsx
@@ -65,6 +65,9 @@
     <t>70</t>
   </si>
   <si>
+    <t>13</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
@@ -117,9 +120,6 @@
   </si>
   <si>
     <t>accessMembers()</t>
-  </si>
-  <si>
-    <t>0</t>
   </si>
 </sst>
 </file>
@@ -226,25 +226,25 @@
         <v>16</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="H2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J2" t="s">
         <v>11</v>
       </c>
       <c r="K2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L2"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -253,7 +253,7 @@
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
         <v>15</v>
@@ -262,25 +262,25 @@
         <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="H3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L3"/>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
@@ -289,7 +289,7 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
@@ -298,25 +298,25 @@
         <v>16</v>
       </c>
       <c r="G4" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="H4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J4" t="s">
         <v>11</v>
       </c>
       <c r="K4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L4"/>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
@@ -325,7 +325,7 @@
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
         <v>15</v>
@@ -334,25 +334,25 @@
         <v>16</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="H5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J5" t="s">
         <v>11</v>
       </c>
       <c r="K5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
@@ -361,7 +361,7 @@
         <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s">
         <v>15</v>
@@ -370,25 +370,25 @@
         <v>16</v>
       </c>
       <c r="G6" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="H6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J6" t="s">
         <v>11</v>
       </c>
       <c r="K6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
@@ -397,7 +397,7 @@
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E7" t="s">
         <v>15</v>
@@ -406,19 +406,19 @@
         <v>16</v>
       </c>
       <c r="G7" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="H7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J7" t="s">
         <v>11</v>
       </c>
       <c r="K7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L7"/>
     </row>
@@ -433,7 +433,7 @@
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E8" t="s">
         <v>15</v>
@@ -442,55 +442,55 @@
         <v>16</v>
       </c>
       <c r="G8" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="H8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L8"/>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E9" t="s">
         <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G9" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="H9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J9" t="s">
         <v>11</v>
       </c>
       <c r="K9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L9"/>
     </row>

</xml_diff>